<commit_message>
added the -2 to 5 interval window
</commit_message>
<xml_diff>
--- a/Summary_MM10.xlsx
+++ b/Summary_MM10.xlsx
@@ -1122,8 +1122,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100147073C54AC26F4FB79B908A17AC475B" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f99071ebfb5f9602e001f3c8275bd3f1">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="60580afd-2765-415e-a024-7e9ff761332b" xmlns:ns3="33819ea0-ebe2-49a1-a511-2fdfd15f8040" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="18b3f5ff91d0997a09a64edcf4beb1df" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100147073C54AC26F4FB79B908A17AC475B" ma:contentTypeVersion="15" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="bb590998a44ab88fea0650574a73f554">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="60580afd-2765-415e-a024-7e9ff761332b" xmlns:ns3="33819ea0-ebe2-49a1-a511-2fdfd15f8040" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="20193022e6678c770d54d851a8531e65" ns2:_="" ns3:_="">
     <xsd:import namespace="60580afd-2765-415e-a024-7e9ff761332b"/>
     <xsd:import namespace="33819ea0-ebe2-49a1-a511-2fdfd15f8040"/>
     <xsd:element name="properties">
@@ -1210,7 +1210,7 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="19" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="0fb7a9c4-9a8b-4167-8a0f-2d2540a67809" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="19" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Bildmarkierungen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="0fb7a9c4-9a8b-4167-8a0f-2d2540a67809" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -1252,8 +1252,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhaltstyp"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -1363,22 +1363,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0325D16-FC2A-4CD2-9426-C4D4E8236B88}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="60580afd-2765-415e-a024-7e9ff761332b"/>
-    <ds:schemaRef ds:uri="33819ea0-ebe2-49a1-a511-2fdfd15f8040"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB3ABA8D-AF27-4B3B-ADEC-6EEDBA1B40C8}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>